<commit_message>
table headers begin with capital
</commit_message>
<xml_diff>
--- a/data/class_sizes.xlsx
+++ b/data/class_sizes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\corona-college\corona-college\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\corona-college\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6195DBA-13EF-439B-A1FE-0DA6C5F78709}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F527EB88-B274-45FF-AD9E-B01A4D54E095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{84FEA3A4-783B-49BD-B3E4-E541D9EF1174}"/>
   </bookViews>
@@ -89,21 +89,6 @@
     <t>ECO 355</t>
   </si>
   <si>
-    <t>in_person</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>class</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>semester</t>
-  </si>
-  <si>
     <t>Honors College</t>
   </si>
   <si>
@@ -125,9 +110,6 @@
     <t xml:space="preserve">Mathematics </t>
   </si>
   <si>
-    <t>department</t>
-  </si>
-  <si>
     <t>Fall_19</t>
   </si>
   <si>
@@ -138,6 +120,24 @@
   </si>
   <si>
     <t>Winter_20</t>
+  </si>
+  <si>
+    <t>Semester</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>In_person</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,27 +512,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>2018</v>
@@ -541,7 +541,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E2">
         <v>25</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>2018</v>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E3">
         <v>26</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>2018</v>
@@ -581,7 +581,7 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>96</v>
@@ -592,7 +592,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>2018</v>
@@ -601,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>23</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B6">
         <v>2018</v>
@@ -621,7 +621,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E6">
         <v>32</v>
@@ -632,7 +632,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>2018</v>
@@ -641,7 +641,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>38</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>2019</v>
@@ -661,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E8">
         <v>25</v>
@@ -672,7 +672,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>2019</v>
@@ -681,7 +681,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E9">
         <v>23</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>2019</v>
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <v>39</v>
@@ -712,7 +712,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>2019</v>
@@ -721,7 +721,7 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>2019</v>
@@ -741,7 +741,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>39</v>
@@ -752,7 +752,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -761,7 +761,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>2019</v>
@@ -781,7 +781,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>30</v>
@@ -792,7 +792,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>2019</v>
@@ -801,7 +801,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E15">
         <v>39</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B16">
         <v>2019</v>
@@ -821,7 +821,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E16">
         <v>27</v>
@@ -832,7 +832,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>2020</v>
@@ -841,7 +841,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E17">
         <v>29</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B18">
         <v>2020</v>
@@ -861,7 +861,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E18">
         <v>29</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>2020</v>
@@ -881,7 +881,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>40</v>
@@ -892,7 +892,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B20">
         <v>2020</v>
@@ -901,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E20">
         <v>21</v>
@@ -912,7 +912,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>2020</v>
@@ -921,7 +921,7 @@
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E21">
         <v>40</v>

</xml_diff>